<commit_message>
Agile docs sprint 3
</commit_message>
<xml_diff>
--- a/_sprints/sprint3/burndown/Sprint 3 Burndown Chart Version 0.xlsx
+++ b/_sprints/sprint3/burndown/Sprint 3 Burndown Chart Version 0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Grad School\Emerging Processes\adventra-app\_sprints\sprint3\burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95BF940-F878-45B8-96EF-755DC79F0F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9322C319-8C9A-4BC4-9616-10B6E9352732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5E7660C9-43B9-406B-90F3-620F8B00C16F}"/>
+    <workbookView xWindow="7200" yWindow="1185" windowWidth="21600" windowHeight="11295" xr2:uid="{5E7660C9-43B9-406B-90F3-620F8B00C16F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,6 +282,33 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -388,55 +415,55 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.941176470588236</c:v>
+                  <c:v>47.058823529411768</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.882352941176471</c:v>
+                  <c:v>44.117647058823529</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.823529411764707</c:v>
+                  <c:v>41.17647058823529</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.764705882352942</c:v>
+                  <c:v>38.235294117647058</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.705882352941178</c:v>
+                  <c:v>35.294117647058826</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.647058823529413</c:v>
+                  <c:v>32.352941176470587</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.588235294117647</c:v>
+                  <c:v>29.411764705882351</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5294117647058822</c:v>
+                  <c:v>26.470588235294116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.4705882352941178</c:v>
+                  <c:v>23.529411764705884</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4117647058823533</c:v>
+                  <c:v>20.588235294117649</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.3529411764705888</c:v>
+                  <c:v>17.647058823529413</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2941176470588243</c:v>
+                  <c:v>14.705882352941174</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.235294117647058</c:v>
+                  <c:v>11.764705882352942</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1764705882352935</c:v>
+                  <c:v>8.823529411764703</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.117647058823529</c:v>
+                  <c:v>5.882352941176471</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0588235294117645</c:v>
+                  <c:v>2.941176470588232</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -564,7 +591,7 @@
         <c:axId val="1203719647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="18"/>
+          <c:max val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -643,7 +670,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1262,15 +1289,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>607218</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>169067</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>583406</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1597,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2833B33-3F9B-43E4-AB7A-DBE02589F971}">
   <dimension ref="C6:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,9 +1655,12 @@
       <c r="D7" s="2">
         <v>1</v>
       </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
       <c r="F7" s="3">
-        <f>18 - (18*(D7-1)/17)</f>
-        <v>18</v>
+        <f t="shared" ref="F7:F24" si="0">50 - (50*(D7-1)/17)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
@@ -1640,9 +1670,12 @@
       <c r="D8" s="2">
         <v>2</v>
       </c>
+      <c r="E8">
+        <v>50</v>
+      </c>
       <c r="F8" s="3">
-        <f>18 - (18*(D8-1)/17)</f>
-        <v>16.941176470588236</v>
+        <f t="shared" si="0"/>
+        <v>47.058823529411768</v>
       </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
@@ -1652,9 +1685,12 @@
       <c r="D9" s="2">
         <v>3</v>
       </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
       <c r="F9" s="3">
-        <f>18 - (18*(D9-1)/17)</f>
-        <v>15.882352941176471</v>
+        <f t="shared" si="0"/>
+        <v>44.117647058823529</v>
       </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
@@ -1664,9 +1700,12 @@
       <c r="D10" s="2">
         <v>4</v>
       </c>
+      <c r="E10">
+        <v>50</v>
+      </c>
       <c r="F10" s="3">
-        <f>18 - (18*(D10-1)/17)</f>
-        <v>14.823529411764707</v>
+        <f t="shared" si="0"/>
+        <v>41.17647058823529</v>
       </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.25">
@@ -1676,9 +1715,12 @@
       <c r="D11" s="2">
         <v>5</v>
       </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
       <c r="F11" s="3">
-        <f>18 - (18*(D11-1)/17)</f>
-        <v>13.764705882352942</v>
+        <f t="shared" si="0"/>
+        <v>38.235294117647058</v>
       </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
@@ -1688,9 +1730,12 @@
       <c r="D12" s="2">
         <v>6</v>
       </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
       <c r="F12" s="3">
-        <f>18 - (18*(D12-1)/17)</f>
-        <v>12.705882352941178</v>
+        <f t="shared" si="0"/>
+        <v>35.294117647058826</v>
       </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
@@ -1700,9 +1745,12 @@
       <c r="D13" s="2">
         <v>7</v>
       </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
       <c r="F13" s="3">
-        <f>18 - (18*(D13-1)/17)</f>
-        <v>11.647058823529413</v>
+        <f t="shared" si="0"/>
+        <v>32.352941176470587</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
@@ -1712,9 +1760,12 @@
       <c r="D14" s="2">
         <v>8</v>
       </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
       <c r="F14" s="3">
-        <f>18 - (18*(D14-1)/17)</f>
-        <v>10.588235294117647</v>
+        <f t="shared" si="0"/>
+        <v>29.411764705882351</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
@@ -1724,9 +1775,12 @@
       <c r="D15" s="2">
         <v>9</v>
       </c>
+      <c r="E15">
+        <v>50</v>
+      </c>
       <c r="F15" s="3">
-        <f>18 - (18*(D15-1)/17)</f>
-        <v>9.5294117647058822</v>
+        <f t="shared" si="0"/>
+        <v>26.470588235294116</v>
       </c>
       <c r="T15" t="s">
         <v>4</v>
@@ -1740,8 +1794,8 @@
         <v>10</v>
       </c>
       <c r="F16" s="3">
-        <f>18 - (18*(D16-1)/17)</f>
-        <v>8.4705882352941178</v>
+        <f t="shared" si="0"/>
+        <v>23.529411764705884</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
@@ -1752,8 +1806,8 @@
         <v>11</v>
       </c>
       <c r="F17" s="3">
-        <f>18 - (18*(D17-1)/17)</f>
-        <v>7.4117647058823533</v>
+        <f t="shared" si="0"/>
+        <v>20.588235294117649</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
@@ -1764,8 +1818,8 @@
         <v>12</v>
       </c>
       <c r="F18" s="3">
-        <f>18 - (18*(D18-1)/17)</f>
-        <v>6.3529411764705888</v>
+        <f t="shared" si="0"/>
+        <v>17.647058823529413</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
@@ -1776,8 +1830,8 @@
         <v>13</v>
       </c>
       <c r="F19" s="3">
-        <f>18 - (18*(D19-1)/17)</f>
-        <v>5.2941176470588243</v>
+        <f t="shared" si="0"/>
+        <v>14.705882352941174</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
@@ -1788,8 +1842,8 @@
         <v>14</v>
       </c>
       <c r="F20" s="3">
-        <f>18 - (18*(D20-1)/17)</f>
-        <v>4.235294117647058</v>
+        <f t="shared" si="0"/>
+        <v>11.764705882352942</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
@@ -1800,8 +1854,8 @@
         <v>15</v>
       </c>
       <c r="F21" s="3">
-        <f>18 - (18*(D21-1)/17)</f>
-        <v>3.1764705882352935</v>
+        <f t="shared" si="0"/>
+        <v>8.823529411764703</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -1812,8 +1866,8 @@
         <v>16</v>
       </c>
       <c r="F22" s="3">
-        <f>18 - (18*(D22-1)/17)</f>
-        <v>2.117647058823529</v>
+        <f t="shared" si="0"/>
+        <v>5.882352941176471</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
@@ -1824,8 +1878,8 @@
         <v>17</v>
       </c>
       <c r="F23" s="3">
-        <f>18 - (18*(D23-1)/17)</f>
-        <v>1.0588235294117645</v>
+        <f t="shared" si="0"/>
+        <v>2.941176470588232</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
@@ -1836,7 +1890,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="3">
-        <f>18 - (18*(D24-1)/17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>